<commit_message>
Upload data and R script
</commit_message>
<xml_diff>
--- a/Q12_Propoerty Rights and Rule-based Governance.xlsx
+++ b/Q12_Propoerty Rights and Rule-based Governance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb533078\OneDrive - WBG\2 VISUAL AND CONTENT\REPORTS\Q12_Propoerty Rights and Rule-based Governance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb533078\Documents\Work Repositories\GovData_Property_Rights_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>Institutional Profiles Database 2016</t>
   </si>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,6 +641,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>290</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
@@ -652,6 +655,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2763</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
@@ -660,6 +666,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>291</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
@@ -668,6 +677,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>294</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
@@ -689,6 +701,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>747</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
@@ -697,6 +712,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>476</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
@@ -705,6 +723,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>477</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
@@ -713,6 +734,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>478</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
@@ -721,6 +745,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>468</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
@@ -729,6 +756,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>470</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
@@ -737,6 +767,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>471</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
@@ -744,7 +777,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>472</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
@@ -752,7 +788,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>473</v>
+      </c>
       <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
@@ -760,7 +799,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>28828</v>
+      </c>
       <c r="B19" s="10" t="s">
         <v>45</v>
       </c>
@@ -768,11 +810,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
@@ -780,7 +822,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>370</v>
+      </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -788,7 +833,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>21</v>
       </c>
@@ -802,20 +847,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>27881</v>
+      </c>
       <c r="B25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>27882</v>
+      </c>
       <c r="B26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
+      <c r="C26" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>6</v>
@@ -824,19 +877,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27897</v>
+      </c>
       <c r="B27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
+      <c r="C27" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27914</v>
+      </c>
       <c r="B28" s="1" t="s">
         <v>22</v>
       </c>
@@ -846,7 +905,10 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27926</v>
+      </c>
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
@@ -856,12 +918,12 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>0</v>
       </c>
@@ -871,7 +933,7 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
@@ -960,8 +1022,11 @@
     <hyperlink ref="C35" r:id="rId17"/>
     <hyperlink ref="C36" r:id="rId18"/>
     <hyperlink ref="C37" r:id="rId19"/>
+    <hyperlink ref="C25" r:id="rId20"/>
+    <hyperlink ref="C26" r:id="rId21"/>
+    <hyperlink ref="C27" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Data and message for the future.
</commit_message>
<xml_diff>
--- a/Q12_Propoerty Rights and Rule-based Governance.xlsx
+++ b/Q12_Propoerty Rights and Rule-based Governance.xlsx
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>